<commit_message>
Fix session persistence bug and update Finance Required bucket mappings
</commit_message>
<xml_diff>
--- a/marquette_courses_full.xlsx
+++ b/marquette_courses_full.xlsx
@@ -3779,14 +3779,14 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Core Required</t>
+          <t>Finance Required</t>
         </is>
       </c>
       <c r="D2" t="n">
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
@@ -3893,7 +3893,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F72"/>
+  <dimension ref="A1:F91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5101,16 +5101,16 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>CORE</t>
+          <t>BUS_ELEC_4</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>ECON 1103</t>
+          <t>FINA 3002</t>
         </is>
       </c>
       <c r="D50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E50" t="b">
         <v>1</v>
@@ -5125,16 +5125,16 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>CORE</t>
+          <t>BUS_ELEC_4</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>ECON 1104</t>
+          <t>FINA 4002</t>
         </is>
       </c>
       <c r="D51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E51" t="b">
         <v>1</v>
@@ -5154,7 +5154,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>FINA 3002</t>
+          <t>FINA 4020</t>
         </is>
       </c>
       <c r="D52" t="b">
@@ -5178,7 +5178,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>FINA 4002</t>
+          <t>FINA 4023</t>
         </is>
       </c>
       <c r="D53" t="b">
@@ -5202,7 +5202,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>FINA 4020</t>
+          <t>FINA 4040</t>
         </is>
       </c>
       <c r="D54" t="b">
@@ -5226,7 +5226,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>FINA 4023</t>
+          <t>FINA 4050</t>
         </is>
       </c>
       <c r="D55" t="b">
@@ -5250,7 +5250,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>FINA 4040</t>
+          <t>FINA 4060</t>
         </is>
       </c>
       <c r="D56" t="b">
@@ -5274,7 +5274,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>FINA 4050</t>
+          <t>FINA 4065</t>
         </is>
       </c>
       <c r="D57" t="b">
@@ -5298,7 +5298,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>FINA 4060</t>
+          <t>FINA 4075</t>
         </is>
       </c>
       <c r="D58" t="b">
@@ -5322,7 +5322,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>FINA 4065</t>
+          <t>FINA 4081</t>
         </is>
       </c>
       <c r="D59" t="b">
@@ -5346,7 +5346,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>FINA 4075</t>
+          <t>FINA 4082</t>
         </is>
       </c>
       <c r="D60" t="b">
@@ -5370,7 +5370,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>FINA 4081</t>
+          <t>FINA 4084</t>
         </is>
       </c>
       <c r="D61" t="b">
@@ -5394,7 +5394,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>FINA 4082</t>
+          <t>FINA 4085</t>
         </is>
       </c>
       <c r="D62" t="b">
@@ -5418,7 +5418,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>FINA 4084</t>
+          <t>FINA 4191</t>
         </is>
       </c>
       <c r="D63" t="b">
@@ -5442,7 +5442,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>FINA 4085</t>
+          <t>FINA 4210</t>
         </is>
       </c>
       <c r="D64" t="b">
@@ -5466,7 +5466,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>FINA 4191</t>
+          <t>FINA 4211</t>
         </is>
       </c>
       <c r="D65" t="b">
@@ -5490,7 +5490,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>FINA 4210</t>
+          <t>FINA 4212</t>
         </is>
       </c>
       <c r="D66" t="b">
@@ -5514,7 +5514,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>FINA 4211</t>
+          <t>FINA 4931</t>
         </is>
       </c>
       <c r="D67" t="b">
@@ -5538,7 +5538,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>FINA 4212</t>
+          <t>FINA 4953</t>
         </is>
       </c>
       <c r="D68" t="b">
@@ -5562,7 +5562,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>FINA 4931</t>
+          <t>FINA 4986</t>
         </is>
       </c>
       <c r="D69" t="b">
@@ -5586,7 +5586,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>FINA 4953</t>
+          <t>FINA 4989</t>
         </is>
       </c>
       <c r="D70" t="b">
@@ -5605,16 +5605,16 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>BUS_ELEC_4</t>
+          <t>CORE</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>FINA 4986</t>
+          <t>FINA 3002</t>
         </is>
       </c>
       <c r="D71" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E71" t="b">
         <v>1</v>
@@ -5629,21 +5629,477 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>BUS_ELEC_4</t>
+          <t>CORE</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
+          <t>FINA 4002</t>
+        </is>
+      </c>
+      <c r="D72" t="b">
+        <v>1</v>
+      </c>
+      <c r="E72" t="b">
+        <v>1</v>
+      </c>
+      <c r="F72" t="inlineStr"/>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>FINA 4020</t>
+        </is>
+      </c>
+      <c r="D73" t="b">
+        <v>1</v>
+      </c>
+      <c r="E73" t="b">
+        <v>1</v>
+      </c>
+      <c r="F73" t="inlineStr"/>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>FINA 4023</t>
+        </is>
+      </c>
+      <c r="D74" t="b">
+        <v>1</v>
+      </c>
+      <c r="E74" t="b">
+        <v>1</v>
+      </c>
+      <c r="F74" t="inlineStr"/>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>FINA 4040</t>
+        </is>
+      </c>
+      <c r="D75" t="b">
+        <v>1</v>
+      </c>
+      <c r="E75" t="b">
+        <v>1</v>
+      </c>
+      <c r="F75" t="inlineStr"/>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>FINA 4050</t>
+        </is>
+      </c>
+      <c r="D76" t="b">
+        <v>1</v>
+      </c>
+      <c r="E76" t="b">
+        <v>1</v>
+      </c>
+      <c r="F76" t="inlineStr"/>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>FINA 4060</t>
+        </is>
+      </c>
+      <c r="D77" t="b">
+        <v>1</v>
+      </c>
+      <c r="E77" t="b">
+        <v>1</v>
+      </c>
+      <c r="F77" t="inlineStr"/>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>FINA 4065</t>
+        </is>
+      </c>
+      <c r="D78" t="b">
+        <v>1</v>
+      </c>
+      <c r="E78" t="b">
+        <v>1</v>
+      </c>
+      <c r="F78" t="inlineStr"/>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>FINA 4075</t>
+        </is>
+      </c>
+      <c r="D79" t="b">
+        <v>1</v>
+      </c>
+      <c r="E79" t="b">
+        <v>1</v>
+      </c>
+      <c r="F79" t="inlineStr"/>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>FINA 4081</t>
+        </is>
+      </c>
+      <c r="D80" t="b">
+        <v>1</v>
+      </c>
+      <c r="E80" t="b">
+        <v>1</v>
+      </c>
+      <c r="F80" t="inlineStr"/>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>FINA 4082</t>
+        </is>
+      </c>
+      <c r="D81" t="b">
+        <v>1</v>
+      </c>
+      <c r="E81" t="b">
+        <v>1</v>
+      </c>
+      <c r="F81" t="inlineStr"/>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>FINA 4084</t>
+        </is>
+      </c>
+      <c r="D82" t="b">
+        <v>1</v>
+      </c>
+      <c r="E82" t="b">
+        <v>1</v>
+      </c>
+      <c r="F82" t="inlineStr"/>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>FINA 4085</t>
+        </is>
+      </c>
+      <c r="D83" t="b">
+        <v>1</v>
+      </c>
+      <c r="E83" t="b">
+        <v>1</v>
+      </c>
+      <c r="F83" t="inlineStr"/>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>FINA 4191</t>
+        </is>
+      </c>
+      <c r="D84" t="b">
+        <v>1</v>
+      </c>
+      <c r="E84" t="b">
+        <v>1</v>
+      </c>
+      <c r="F84" t="inlineStr"/>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>FINA 4210</t>
+        </is>
+      </c>
+      <c r="D85" t="b">
+        <v>1</v>
+      </c>
+      <c r="E85" t="b">
+        <v>1</v>
+      </c>
+      <c r="F85" t="inlineStr"/>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>FINA 4211</t>
+        </is>
+      </c>
+      <c r="D86" t="b">
+        <v>1</v>
+      </c>
+      <c r="E86" t="b">
+        <v>1</v>
+      </c>
+      <c r="F86" t="inlineStr"/>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>FINA 4212</t>
+        </is>
+      </c>
+      <c r="D87" t="b">
+        <v>1</v>
+      </c>
+      <c r="E87" t="b">
+        <v>1</v>
+      </c>
+      <c r="F87" t="inlineStr"/>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>FINA 4931</t>
+        </is>
+      </c>
+      <c r="D88" t="b">
+        <v>1</v>
+      </c>
+      <c r="E88" t="b">
+        <v>1</v>
+      </c>
+      <c r="F88" t="inlineStr"/>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>FINA 4953</t>
+        </is>
+      </c>
+      <c r="D89" t="b">
+        <v>1</v>
+      </c>
+      <c r="E89" t="b">
+        <v>1</v>
+      </c>
+      <c r="F89" t="inlineStr"/>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>FINA 4986</t>
+        </is>
+      </c>
+      <c r="D90" t="b">
+        <v>1</v>
+      </c>
+      <c r="E90" t="b">
+        <v>1</v>
+      </c>
+      <c r="F90" t="inlineStr"/>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
           <t>FINA 4989</t>
         </is>
       </c>
-      <c r="D72" t="b">
-        <v>0</v>
-      </c>
-      <c r="E72" t="b">
-        <v>1</v>
-      </c>
-      <c r="F72" t="inlineStr"/>
+      <c r="D91" t="b">
+        <v>1</v>
+      </c>
+      <c r="E91" t="b">
+        <v>1</v>
+      </c>
+      <c r="F91" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Polish recommendation logic, UI, and course data
</commit_message>
<xml_diff>
--- a/marquette_courses_full.xlsx
+++ b/marquette_courses_full.xlsx
@@ -11,8 +11,7 @@
     <sheet name="equivalencies" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="tracks" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="buckets" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="bucket_course_map" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="README" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="README" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -418,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P45"/>
+  <dimension ref="A1:T45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -507,6 +506,26 @@
           <t>prereq_tier</t>
         </is>
       </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>bucket1</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>bucket2</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>bucket3</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>bucket4</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -569,6 +588,14 @@
           <t>level_0</t>
         </is>
       </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -631,6 +658,14 @@
           <t>level_1</t>
         </is>
       </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -697,6 +732,14 @@
           <t>level_0</t>
         </is>
       </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -759,6 +802,10 @@
           <t>level_0</t>
         </is>
       </c>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -821,6 +868,14 @@
           <t>level_0</t>
         </is>
       </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -883,6 +938,14 @@
           <t>level_1</t>
         </is>
       </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -949,6 +1012,10 @@
           <t>level_0</t>
         </is>
       </c>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
+      <c r="T8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1015,6 +1082,10 @@
           <t>level_0</t>
         </is>
       </c>
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1081,6 +1152,10 @@
           <t>level_1</t>
         </is>
       </c>
+      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr"/>
+      <c r="T10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1147,6 +1222,10 @@
           <t>level_1</t>
         </is>
       </c>
+      <c r="Q11" t="inlineStr"/>
+      <c r="R11" t="inlineStr"/>
+      <c r="S11" t="inlineStr"/>
+      <c r="T11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1209,6 +1288,14 @@
           <t>level_2</t>
         </is>
       </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr"/>
+      <c r="S12" t="inlineStr"/>
+      <c r="T12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1275,6 +1362,14 @@
           <t>level_1</t>
         </is>
       </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" t="inlineStr"/>
+      <c r="T13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1341,6 +1436,10 @@
           <t>level_0</t>
         </is>
       </c>
+      <c r="Q14" t="inlineStr"/>
+      <c r="R14" t="inlineStr"/>
+      <c r="S14" t="inlineStr"/>
+      <c r="T14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1407,6 +1506,10 @@
           <t>level_1</t>
         </is>
       </c>
+      <c r="Q15" t="inlineStr"/>
+      <c r="R15" t="inlineStr"/>
+      <c r="S15" t="inlineStr"/>
+      <c r="T15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1477,6 +1580,14 @@
           <t>level_2</t>
         </is>
       </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr"/>
+      <c r="S16" t="inlineStr"/>
+      <c r="T16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1543,6 +1654,26 @@
           <t>level_3</t>
         </is>
       </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1609,6 +1740,14 @@
           <t>level_0</t>
         </is>
       </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>GENERAL_ELEC</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" t="inlineStr"/>
+      <c r="T18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1675,6 +1814,14 @@
           <t>level_3</t>
         </is>
       </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>GENERAL_ELEC</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr"/>
+      <c r="S19" t="inlineStr"/>
+      <c r="T19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1737,6 +1884,14 @@
           <t>level_3</t>
         </is>
       </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr"/>
+      <c r="S20" t="inlineStr"/>
+      <c r="T20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1799,6 +1954,26 @@
           <t>level_3</t>
         </is>
       </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1861,6 +2036,14 @@
           <t>level_3</t>
         </is>
       </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr"/>
+      <c r="S22" t="inlineStr"/>
+      <c r="T22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1923,6 +2106,26 @@
           <t>level_3</t>
         </is>
       </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1985,6 +2188,26 @@
           <t>level_3</t>
         </is>
       </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+      <c r="T24" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2047,6 +2270,26 @@
           <t>level_3</t>
         </is>
       </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+      <c r="T25" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2109,6 +2352,26 @@
           <t>level_3</t>
         </is>
       </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+      <c r="T26" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2171,6 +2434,26 @@
           <t>level_3</t>
         </is>
       </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+      <c r="T27" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2233,6 +2516,26 @@
           <t>level_3</t>
         </is>
       </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+      <c r="T28" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2295,6 +2598,26 @@
           <t>level_3</t>
         </is>
       </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+      <c r="T29" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2357,6 +2680,26 @@
           <t>level_4</t>
         </is>
       </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+      <c r="S30" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+      <c r="T30" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2419,6 +2762,26 @@
           <t>level_3</t>
         </is>
       </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+      <c r="S31" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+      <c r="T31" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2481,6 +2844,26 @@
           <t>level_3</t>
         </is>
       </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+      <c r="S32" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+      <c r="T32" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2547,6 +2930,26 @@
           <t>level_4</t>
         </is>
       </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+      <c r="S33" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+      <c r="T33" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2609,6 +3012,14 @@
           <t>level_3</t>
         </is>
       </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>GENERAL_ELEC</t>
+        </is>
+      </c>
+      <c r="R34" t="inlineStr"/>
+      <c r="S34" t="inlineStr"/>
+      <c r="T34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2671,6 +3082,14 @@
           <t>level_3</t>
         </is>
       </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>GENERAL_ELEC</t>
+        </is>
+      </c>
+      <c r="R35" t="inlineStr"/>
+      <c r="S35" t="inlineStr"/>
+      <c r="T35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2733,6 +3152,14 @@
           <t>level_4</t>
         </is>
       </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>GENERAL_ELEC</t>
+        </is>
+      </c>
+      <c r="R36" t="inlineStr"/>
+      <c r="S36" t="inlineStr"/>
+      <c r="T36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2795,6 +3222,22 @@
           <t>level_3</t>
         </is>
       </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+      <c r="S37" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+      <c r="T37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2865,6 +3308,26 @@
           <t>level_3</t>
         </is>
       </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+      <c r="S38" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+      <c r="T38" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2931,6 +3394,26 @@
           <t>level_4</t>
         </is>
       </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+      <c r="S39" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+      <c r="T39" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2993,6 +3476,26 @@
           <t>level_4</t>
         </is>
       </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+      <c r="S40" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+      <c r="T40" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -3055,6 +3558,26 @@
           <t>level_3</t>
         </is>
       </c>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+      <c r="S41" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+      <c r="T41" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -3117,6 +3640,22 @@
           <t>level_3</t>
         </is>
       </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="R42" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+      <c r="S42" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+      <c r="T42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -3183,6 +3722,22 @@
           <t>level_4</t>
         </is>
       </c>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="R43" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+      <c r="S43" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+      <c r="T43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -3249,6 +3804,22 @@
           <t>level_3</t>
         </is>
       </c>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+      <c r="S44" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+      <c r="T44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -3315,6 +3886,14 @@
           <t>level_0</t>
         </is>
       </c>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>GENERAL_ELEC</t>
+        </is>
+      </c>
+      <c r="R45" t="inlineStr"/>
+      <c r="S45" t="inlineStr"/>
+      <c r="T45" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3716,7 +4295,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3783,7 +4362,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" t="n">
         <v>6</v>
@@ -3811,7 +4390,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3" t="n">
         <v>2</v>
@@ -3841,7 +4420,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E4" t="n">
         <v>1</v>
@@ -3867,11 +4446,11 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Business Electives</t>
+          <t>Business Core</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
         <v>4</v>
@@ -3880,6 +4459,32 @@
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>GENERAL_ELEC</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>General Elective</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>99</v>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3888,2225 +4493,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F91"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>program_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>bucket_id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>course_code</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>is_required</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>can_double_count</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>constraints</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>CORE</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>FINA 3001</t>
-        </is>
-      </c>
-      <c r="D2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>CORE</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>FINA 4001</t>
-        </is>
-      </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>equiv_group:EQUIV_FINA_4001</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>CORE</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>FINA 4011</t>
-        </is>
-      </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>equiv_group:EQUIV_FINA_4011</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_2</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>FINA 3002</t>
-        </is>
-      </c>
-      <c r="D5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_2</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>FINA 4002</t>
-        </is>
-      </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_2</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>FINA 4020</t>
-        </is>
-      </c>
-      <c r="D7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_2</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>FINA 4023</t>
-        </is>
-      </c>
-      <c r="D8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_2</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>FINA 4040</t>
-        </is>
-      </c>
-      <c r="D9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" t="b">
-        <v>1</v>
-      </c>
-      <c r="F9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_2</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>FINA 4050</t>
-        </is>
-      </c>
-      <c r="D10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_2</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>FINA 4060</t>
-        </is>
-      </c>
-      <c r="D11" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_2</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>FINA 4065</t>
-        </is>
-      </c>
-      <c r="D12" t="b">
-        <v>0</v>
-      </c>
-      <c r="E12" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_2</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>FINA 4075</t>
-        </is>
-      </c>
-      <c r="D13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_2</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>FINA 4081</t>
-        </is>
-      </c>
-      <c r="D14" t="b">
-        <v>0</v>
-      </c>
-      <c r="E14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_2</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>FINA 4082</t>
-        </is>
-      </c>
-      <c r="D15" t="b">
-        <v>0</v>
-      </c>
-      <c r="E15" t="b">
-        <v>1</v>
-      </c>
-      <c r="F15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_2</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>FINA 4084</t>
-        </is>
-      </c>
-      <c r="D16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_2</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>FINA 4085</t>
-        </is>
-      </c>
-      <c r="D17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F17" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_2</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>FINA 4191</t>
-        </is>
-      </c>
-      <c r="D18" t="b">
-        <v>0</v>
-      </c>
-      <c r="E18" t="b">
-        <v>1</v>
-      </c>
-      <c r="F18" t="inlineStr"/>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_2</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>FINA 4210</t>
-        </is>
-      </c>
-      <c r="D19" t="b">
-        <v>0</v>
-      </c>
-      <c r="E19" t="b">
-        <v>1</v>
-      </c>
-      <c r="F19" t="inlineStr"/>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_2</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>FINA 4211</t>
-        </is>
-      </c>
-      <c r="D20" t="b">
-        <v>0</v>
-      </c>
-      <c r="E20" t="b">
-        <v>1</v>
-      </c>
-      <c r="F20" t="inlineStr"/>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_2</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>FINA 4212</t>
-        </is>
-      </c>
-      <c r="D21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E21" t="b">
-        <v>1</v>
-      </c>
-      <c r="F21" t="inlineStr"/>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_2</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>FINA 4931</t>
-        </is>
-      </c>
-      <c r="D22" t="b">
-        <v>0</v>
-      </c>
-      <c r="E22" t="b">
-        <v>1</v>
-      </c>
-      <c r="F22" t="inlineStr"/>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_2</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>FINA 4953</t>
-        </is>
-      </c>
-      <c r="D23" t="b">
-        <v>0</v>
-      </c>
-      <c r="E23" t="b">
-        <v>1</v>
-      </c>
-      <c r="F23" t="inlineStr"/>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_2</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>FINA 4986</t>
-        </is>
-      </c>
-      <c r="D24" t="b">
-        <v>0</v>
-      </c>
-      <c r="E24" t="b">
-        <v>1</v>
-      </c>
-      <c r="F24" t="inlineStr"/>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_2</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>FINA 4989</t>
-        </is>
-      </c>
-      <c r="D25" t="b">
-        <v>0</v>
-      </c>
-      <c r="E25" t="b">
-        <v>1</v>
-      </c>
-      <c r="F25" t="inlineStr"/>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>FINA 3002</t>
-        </is>
-      </c>
-      <c r="D26" t="b">
-        <v>0</v>
-      </c>
-      <c r="E26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F26" t="inlineStr"/>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>FINA 4002</t>
-        </is>
-      </c>
-      <c r="D27" t="b">
-        <v>0</v>
-      </c>
-      <c r="E27" t="b">
-        <v>1</v>
-      </c>
-      <c r="F27" t="inlineStr"/>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>FINA 4020</t>
-        </is>
-      </c>
-      <c r="D28" t="b">
-        <v>0</v>
-      </c>
-      <c r="E28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F28" t="inlineStr"/>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>FINA 4023</t>
-        </is>
-      </c>
-      <c r="D29" t="b">
-        <v>0</v>
-      </c>
-      <c r="E29" t="b">
-        <v>1</v>
-      </c>
-      <c r="F29" t="inlineStr"/>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>FINA 4040</t>
-        </is>
-      </c>
-      <c r="D30" t="b">
-        <v>0</v>
-      </c>
-      <c r="E30" t="b">
-        <v>1</v>
-      </c>
-      <c r="F30" t="inlineStr"/>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>FINA 4050</t>
-        </is>
-      </c>
-      <c r="D31" t="b">
-        <v>0</v>
-      </c>
-      <c r="E31" t="b">
-        <v>1</v>
-      </c>
-      <c r="F31" t="inlineStr"/>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>FINA 4060</t>
-        </is>
-      </c>
-      <c r="D32" t="b">
-        <v>0</v>
-      </c>
-      <c r="E32" t="b">
-        <v>1</v>
-      </c>
-      <c r="F32" t="inlineStr"/>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>FINA 4065</t>
-        </is>
-      </c>
-      <c r="D33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E33" t="b">
-        <v>1</v>
-      </c>
-      <c r="F33" t="inlineStr"/>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>FINA 4075</t>
-        </is>
-      </c>
-      <c r="D34" t="b">
-        <v>0</v>
-      </c>
-      <c r="E34" t="b">
-        <v>1</v>
-      </c>
-      <c r="F34" t="inlineStr"/>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>FINA 4081</t>
-        </is>
-      </c>
-      <c r="D35" t="b">
-        <v>0</v>
-      </c>
-      <c r="E35" t="b">
-        <v>1</v>
-      </c>
-      <c r="F35" t="inlineStr"/>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>FINA 4082</t>
-        </is>
-      </c>
-      <c r="D36" t="b">
-        <v>0</v>
-      </c>
-      <c r="E36" t="b">
-        <v>1</v>
-      </c>
-      <c r="F36" t="inlineStr"/>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>FINA 4084</t>
-        </is>
-      </c>
-      <c r="D37" t="b">
-        <v>0</v>
-      </c>
-      <c r="E37" t="b">
-        <v>1</v>
-      </c>
-      <c r="F37" t="inlineStr"/>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>FINA 4085</t>
-        </is>
-      </c>
-      <c r="D38" t="b">
-        <v>0</v>
-      </c>
-      <c r="E38" t="b">
-        <v>1</v>
-      </c>
-      <c r="F38" t="inlineStr"/>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>FINA 4210</t>
-        </is>
-      </c>
-      <c r="D39" t="b">
-        <v>0</v>
-      </c>
-      <c r="E39" t="b">
-        <v>1</v>
-      </c>
-      <c r="F39" t="inlineStr"/>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>FINA 4211</t>
-        </is>
-      </c>
-      <c r="D40" t="b">
-        <v>0</v>
-      </c>
-      <c r="E40" t="b">
-        <v>1</v>
-      </c>
-      <c r="F40" t="inlineStr"/>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>FINA 4212</t>
-        </is>
-      </c>
-      <c r="D41" t="b">
-        <v>0</v>
-      </c>
-      <c r="E41" t="b">
-        <v>1</v>
-      </c>
-      <c r="F41" t="inlineStr"/>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>FINA 4931</t>
-        </is>
-      </c>
-      <c r="D42" t="b">
-        <v>0</v>
-      </c>
-      <c r="E42" t="b">
-        <v>1</v>
-      </c>
-      <c r="F42" t="inlineStr"/>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>BUS_ELEC_4</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>ACCO 1030</t>
-        </is>
-      </c>
-      <c r="D43" t="b">
-        <v>0</v>
-      </c>
-      <c r="E43" t="b">
-        <v>1</v>
-      </c>
-      <c r="F43" t="inlineStr"/>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>BUS_ELEC_4</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>ACCO 1031</t>
-        </is>
-      </c>
-      <c r="D44" t="b">
-        <v>0</v>
-      </c>
-      <c r="E44" t="b">
-        <v>1</v>
-      </c>
-      <c r="F44" t="inlineStr"/>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>BUS_ELEC_4</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>BUAD 1001</t>
-        </is>
-      </c>
-      <c r="D45" t="b">
-        <v>0</v>
-      </c>
-      <c r="E45" t="b">
-        <v>1</v>
-      </c>
-      <c r="F45" t="inlineStr"/>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>BUS_ELEC_4</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>BUAD 1560</t>
-        </is>
-      </c>
-      <c r="D46" t="b">
-        <v>0</v>
-      </c>
-      <c r="E46" t="b">
-        <v>1</v>
-      </c>
-      <c r="F46" t="inlineStr"/>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>BUS_ELEC_4</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>BUAD 2001</t>
-        </is>
-      </c>
-      <c r="D47" t="b">
-        <v>0</v>
-      </c>
-      <c r="E47" t="b">
-        <v>1</v>
-      </c>
-      <c r="F47" t="inlineStr"/>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>BUS_ELEC_4</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>ECON 1103</t>
-        </is>
-      </c>
-      <c r="D48" t="b">
-        <v>0</v>
-      </c>
-      <c r="E48" t="b">
-        <v>1</v>
-      </c>
-      <c r="F48" t="inlineStr"/>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>BUS_ELEC_4</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>ECON 1104</t>
-        </is>
-      </c>
-      <c r="D49" t="b">
-        <v>0</v>
-      </c>
-      <c r="E49" t="b">
-        <v>1</v>
-      </c>
-      <c r="F49" t="inlineStr"/>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>BUS_ELEC_4</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>FINA 3002</t>
-        </is>
-      </c>
-      <c r="D50" t="b">
-        <v>0</v>
-      </c>
-      <c r="E50" t="b">
-        <v>1</v>
-      </c>
-      <c r="F50" t="inlineStr"/>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>BUS_ELEC_4</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>FINA 4002</t>
-        </is>
-      </c>
-      <c r="D51" t="b">
-        <v>0</v>
-      </c>
-      <c r="E51" t="b">
-        <v>1</v>
-      </c>
-      <c r="F51" t="inlineStr"/>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>BUS_ELEC_4</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>FINA 4020</t>
-        </is>
-      </c>
-      <c r="D52" t="b">
-        <v>0</v>
-      </c>
-      <c r="E52" t="b">
-        <v>1</v>
-      </c>
-      <c r="F52" t="inlineStr"/>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>BUS_ELEC_4</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>FINA 4023</t>
-        </is>
-      </c>
-      <c r="D53" t="b">
-        <v>0</v>
-      </c>
-      <c r="E53" t="b">
-        <v>1</v>
-      </c>
-      <c r="F53" t="inlineStr"/>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>BUS_ELEC_4</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>FINA 4040</t>
-        </is>
-      </c>
-      <c r="D54" t="b">
-        <v>0</v>
-      </c>
-      <c r="E54" t="b">
-        <v>1</v>
-      </c>
-      <c r="F54" t="inlineStr"/>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>BUS_ELEC_4</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>FINA 4050</t>
-        </is>
-      </c>
-      <c r="D55" t="b">
-        <v>0</v>
-      </c>
-      <c r="E55" t="b">
-        <v>1</v>
-      </c>
-      <c r="F55" t="inlineStr"/>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>BUS_ELEC_4</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>FINA 4060</t>
-        </is>
-      </c>
-      <c r="D56" t="b">
-        <v>0</v>
-      </c>
-      <c r="E56" t="b">
-        <v>1</v>
-      </c>
-      <c r="F56" t="inlineStr"/>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>BUS_ELEC_4</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>FINA 4065</t>
-        </is>
-      </c>
-      <c r="D57" t="b">
-        <v>0</v>
-      </c>
-      <c r="E57" t="b">
-        <v>1</v>
-      </c>
-      <c r="F57" t="inlineStr"/>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>BUS_ELEC_4</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>FINA 4075</t>
-        </is>
-      </c>
-      <c r="D58" t="b">
-        <v>0</v>
-      </c>
-      <c r="E58" t="b">
-        <v>1</v>
-      </c>
-      <c r="F58" t="inlineStr"/>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>BUS_ELEC_4</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>FINA 4081</t>
-        </is>
-      </c>
-      <c r="D59" t="b">
-        <v>0</v>
-      </c>
-      <c r="E59" t="b">
-        <v>1</v>
-      </c>
-      <c r="F59" t="inlineStr"/>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>BUS_ELEC_4</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>FINA 4082</t>
-        </is>
-      </c>
-      <c r="D60" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" t="b">
-        <v>1</v>
-      </c>
-      <c r="F60" t="inlineStr"/>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>BUS_ELEC_4</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>FINA 4084</t>
-        </is>
-      </c>
-      <c r="D61" t="b">
-        <v>0</v>
-      </c>
-      <c r="E61" t="b">
-        <v>1</v>
-      </c>
-      <c r="F61" t="inlineStr"/>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>BUS_ELEC_4</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>FINA 4085</t>
-        </is>
-      </c>
-      <c r="D62" t="b">
-        <v>0</v>
-      </c>
-      <c r="E62" t="b">
-        <v>1</v>
-      </c>
-      <c r="F62" t="inlineStr"/>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>BUS_ELEC_4</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>FINA 4191</t>
-        </is>
-      </c>
-      <c r="D63" t="b">
-        <v>0</v>
-      </c>
-      <c r="E63" t="b">
-        <v>1</v>
-      </c>
-      <c r="F63" t="inlineStr"/>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>BUS_ELEC_4</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>FINA 4210</t>
-        </is>
-      </c>
-      <c r="D64" t="b">
-        <v>0</v>
-      </c>
-      <c r="E64" t="b">
-        <v>1</v>
-      </c>
-      <c r="F64" t="inlineStr"/>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>BUS_ELEC_4</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>FINA 4211</t>
-        </is>
-      </c>
-      <c r="D65" t="b">
-        <v>0</v>
-      </c>
-      <c r="E65" t="b">
-        <v>1</v>
-      </c>
-      <c r="F65" t="inlineStr"/>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>BUS_ELEC_4</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>FINA 4212</t>
-        </is>
-      </c>
-      <c r="D66" t="b">
-        <v>0</v>
-      </c>
-      <c r="E66" t="b">
-        <v>1</v>
-      </c>
-      <c r="F66" t="inlineStr"/>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>BUS_ELEC_4</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>FINA 4931</t>
-        </is>
-      </c>
-      <c r="D67" t="b">
-        <v>0</v>
-      </c>
-      <c r="E67" t="b">
-        <v>1</v>
-      </c>
-      <c r="F67" t="inlineStr"/>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>BUS_ELEC_4</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>FINA 4953</t>
-        </is>
-      </c>
-      <c r="D68" t="b">
-        <v>0</v>
-      </c>
-      <c r="E68" t="b">
-        <v>1</v>
-      </c>
-      <c r="F68" t="inlineStr"/>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>BUS_ELEC_4</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>FINA 4986</t>
-        </is>
-      </c>
-      <c r="D69" t="b">
-        <v>0</v>
-      </c>
-      <c r="E69" t="b">
-        <v>1</v>
-      </c>
-      <c r="F69" t="inlineStr"/>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>BUS_ELEC_4</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>FINA 4989</t>
-        </is>
-      </c>
-      <c r="D70" t="b">
-        <v>0</v>
-      </c>
-      <c r="E70" t="b">
-        <v>1</v>
-      </c>
-      <c r="F70" t="inlineStr"/>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>CORE</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>FINA 3002</t>
-        </is>
-      </c>
-      <c r="D71" t="b">
-        <v>1</v>
-      </c>
-      <c r="E71" t="b">
-        <v>1</v>
-      </c>
-      <c r="F71" t="inlineStr"/>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>CORE</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>FINA 4002</t>
-        </is>
-      </c>
-      <c r="D72" t="b">
-        <v>1</v>
-      </c>
-      <c r="E72" t="b">
-        <v>1</v>
-      </c>
-      <c r="F72" t="inlineStr"/>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>CORE</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>FINA 4020</t>
-        </is>
-      </c>
-      <c r="D73" t="b">
-        <v>1</v>
-      </c>
-      <c r="E73" t="b">
-        <v>1</v>
-      </c>
-      <c r="F73" t="inlineStr"/>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>CORE</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>FINA 4023</t>
-        </is>
-      </c>
-      <c r="D74" t="b">
-        <v>1</v>
-      </c>
-      <c r="E74" t="b">
-        <v>1</v>
-      </c>
-      <c r="F74" t="inlineStr"/>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>CORE</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>FINA 4040</t>
-        </is>
-      </c>
-      <c r="D75" t="b">
-        <v>1</v>
-      </c>
-      <c r="E75" t="b">
-        <v>1</v>
-      </c>
-      <c r="F75" t="inlineStr"/>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>CORE</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>FINA 4050</t>
-        </is>
-      </c>
-      <c r="D76" t="b">
-        <v>1</v>
-      </c>
-      <c r="E76" t="b">
-        <v>1</v>
-      </c>
-      <c r="F76" t="inlineStr"/>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>CORE</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>FINA 4060</t>
-        </is>
-      </c>
-      <c r="D77" t="b">
-        <v>1</v>
-      </c>
-      <c r="E77" t="b">
-        <v>1</v>
-      </c>
-      <c r="F77" t="inlineStr"/>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>CORE</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>FINA 4065</t>
-        </is>
-      </c>
-      <c r="D78" t="b">
-        <v>1</v>
-      </c>
-      <c r="E78" t="b">
-        <v>1</v>
-      </c>
-      <c r="F78" t="inlineStr"/>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>CORE</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>FINA 4075</t>
-        </is>
-      </c>
-      <c r="D79" t="b">
-        <v>1</v>
-      </c>
-      <c r="E79" t="b">
-        <v>1</v>
-      </c>
-      <c r="F79" t="inlineStr"/>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>CORE</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>FINA 4081</t>
-        </is>
-      </c>
-      <c r="D80" t="b">
-        <v>1</v>
-      </c>
-      <c r="E80" t="b">
-        <v>1</v>
-      </c>
-      <c r="F80" t="inlineStr"/>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>CORE</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>FINA 4082</t>
-        </is>
-      </c>
-      <c r="D81" t="b">
-        <v>1</v>
-      </c>
-      <c r="E81" t="b">
-        <v>1</v>
-      </c>
-      <c r="F81" t="inlineStr"/>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>CORE</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>FINA 4084</t>
-        </is>
-      </c>
-      <c r="D82" t="b">
-        <v>1</v>
-      </c>
-      <c r="E82" t="b">
-        <v>1</v>
-      </c>
-      <c r="F82" t="inlineStr"/>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>CORE</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>FINA 4085</t>
-        </is>
-      </c>
-      <c r="D83" t="b">
-        <v>1</v>
-      </c>
-      <c r="E83" t="b">
-        <v>1</v>
-      </c>
-      <c r="F83" t="inlineStr"/>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>CORE</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>FINA 4191</t>
-        </is>
-      </c>
-      <c r="D84" t="b">
-        <v>1</v>
-      </c>
-      <c r="E84" t="b">
-        <v>1</v>
-      </c>
-      <c r="F84" t="inlineStr"/>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>CORE</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>FINA 4210</t>
-        </is>
-      </c>
-      <c r="D85" t="b">
-        <v>1</v>
-      </c>
-      <c r="E85" t="b">
-        <v>1</v>
-      </c>
-      <c r="F85" t="inlineStr"/>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>CORE</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>FINA 4211</t>
-        </is>
-      </c>
-      <c r="D86" t="b">
-        <v>1</v>
-      </c>
-      <c r="E86" t="b">
-        <v>1</v>
-      </c>
-      <c r="F86" t="inlineStr"/>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>CORE</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>FINA 4212</t>
-        </is>
-      </c>
-      <c r="D87" t="b">
-        <v>1</v>
-      </c>
-      <c r="E87" t="b">
-        <v>1</v>
-      </c>
-      <c r="F87" t="inlineStr"/>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>CORE</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>FINA 4931</t>
-        </is>
-      </c>
-      <c r="D88" t="b">
-        <v>1</v>
-      </c>
-      <c r="E88" t="b">
-        <v>1</v>
-      </c>
-      <c r="F88" t="inlineStr"/>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>CORE</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>FINA 4953</t>
-        </is>
-      </c>
-      <c r="D89" t="b">
-        <v>1</v>
-      </c>
-      <c r="E89" t="b">
-        <v>1</v>
-      </c>
-      <c r="F89" t="inlineStr"/>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>CORE</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>FINA 4986</t>
-        </is>
-      </c>
-      <c r="D90" t="b">
-        <v>1</v>
-      </c>
-      <c r="E90" t="b">
-        <v>1</v>
-      </c>
-      <c r="F90" t="inlineStr"/>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>FIN_MAJOR</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>CORE</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>FINA 4989</t>
-        </is>
-      </c>
-      <c r="D91" t="b">
-        <v>1</v>
-      </c>
-      <c r="E91" t="b">
-        <v>1</v>
-      </c>
-      <c r="F91" t="inlineStr"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
Normalize course-bucket schema and fix boolean coercion
- Add course_bucket sheet (normalized, 96 rows) to workbook via migrate_schema.py
- Fix _safe_bool_col() to handle int/float/string bool variants (1/0, yes/no, y/n)
- Replace crash-prone bucket map sheet lookup with 4-level fallback chain
- Remove row-level can_double_count gate; double-count now gated by bucket-level allow_double_count only
- Remove can_double_count from eligibility.py get_course_eligible_buckets() return shape
- Raise MAX_BUCKETS_PER_COURSE from 2 to 6
- Add 114 regression tests (test_schema_migration.py) covering bool coercion, loader fallback, double-count
</commit_message>
<xml_diff>
--- a/marquette_courses_full.xlsx
+++ b/marquette_courses_full.xlsx
@@ -12,6 +12,7 @@
     <sheet name="tracks" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="buckets" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="README" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="course_bucket" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -554,7 +555,6 @@
           <t>none</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
       <c r="H2" t="b">
         <v>1</v>
       </c>
@@ -574,7 +574,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr">
         <is>
           <t>none</t>
@@ -593,9 +592,6 @@
           <t>BUS_ELEC_4</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -624,7 +620,6 @@
           <t>ACCO 1030</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
       <c r="H3" t="b">
         <v>1</v>
       </c>
@@ -644,7 +639,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr">
         <is>
           <t>none</t>
@@ -663,9 +657,6 @@
           <t>BUS_ELEC_4</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -718,7 +709,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr">
         <is>
           <t>none</t>
@@ -737,9 +727,6 @@
           <t>BUS_ELEC_4</t>
         </is>
       </c>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -768,7 +755,6 @@
           <t>none</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr"/>
       <c r="H5" t="b">
         <v>1</v>
       </c>
@@ -788,7 +774,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr">
         <is>
           <t>none</t>
@@ -802,10 +787,6 @@
           <t>level_0</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr"/>
-      <c r="T5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -834,7 +815,6 @@
           <t>none</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
       <c r="H6" t="b">
         <v>1</v>
       </c>
@@ -854,7 +834,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr">
         <is>
           <t>none</t>
@@ -873,9 +852,6 @@
           <t>BUS_ELEC_4</t>
         </is>
       </c>
-      <c r="R6" t="inlineStr"/>
-      <c r="S6" t="inlineStr"/>
-      <c r="T6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -904,7 +880,6 @@
           <t>ECON 1103</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
       <c r="H7" t="b">
         <v>1</v>
       </c>
@@ -924,7 +899,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr">
         <is>
           <t>none</t>
@@ -943,9 +917,6 @@
           <t>BUS_ELEC_4</t>
         </is>
       </c>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr"/>
-      <c r="T7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -998,7 +969,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr">
         <is>
           <t>none</t>
@@ -1012,10 +982,6 @@
           <t>level_0</t>
         </is>
       </c>
-      <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="inlineStr"/>
-      <c r="S8" t="inlineStr"/>
-      <c r="T8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1068,7 +1034,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr">
         <is>
           <t>none</t>
@@ -1082,10 +1047,6 @@
           <t>level_0</t>
         </is>
       </c>
-      <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="inlineStr"/>
-      <c r="S9" t="inlineStr"/>
-      <c r="T9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1138,7 +1099,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr">
         <is>
           <t>none</t>
@@ -1152,10 +1112,6 @@
           <t>level_1</t>
         </is>
       </c>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" t="inlineStr"/>
-      <c r="T10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1208,7 +1164,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr">
         <is>
           <t>none</t>
@@ -1222,10 +1177,6 @@
           <t>level_1</t>
         </is>
       </c>
-      <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="inlineStr"/>
-      <c r="S11" t="inlineStr"/>
-      <c r="T11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1254,7 +1205,6 @@
           <t>MATH 1400 or MATH 1450</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr"/>
       <c r="H12" t="b">
         <v>1</v>
       </c>
@@ -1274,7 +1224,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr">
         <is>
           <t>none</t>
@@ -1293,9 +1242,6 @@
           <t>BUS_ELEC_4</t>
         </is>
       </c>
-      <c r="R12" t="inlineStr"/>
-      <c r="S12" t="inlineStr"/>
-      <c r="T12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1348,7 +1294,6 @@
           <t>low</t>
         </is>
       </c>
-      <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr">
         <is>
           <t>BUAD 1560</t>
@@ -1367,9 +1312,6 @@
           <t>BUS_ELEC_4</t>
         </is>
       </c>
-      <c r="R13" t="inlineStr"/>
-      <c r="S13" t="inlineStr"/>
-      <c r="T13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1422,7 +1364,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr">
         <is>
           <t>none</t>
@@ -1436,10 +1377,6 @@
           <t>level_0</t>
         </is>
       </c>
-      <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="inlineStr"/>
-      <c r="S14" t="inlineStr"/>
-      <c r="T14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1492,7 +1429,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr">
         <is>
           <t>none</t>
@@ -1506,10 +1442,6 @@
           <t>level_1</t>
         </is>
       </c>
-      <c r="Q15" t="inlineStr"/>
-      <c r="R15" t="inlineStr"/>
-      <c r="S15" t="inlineStr"/>
-      <c r="T15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1585,9 +1517,6 @@
           <t>CORE</t>
         </is>
       </c>
-      <c r="R16" t="inlineStr"/>
-      <c r="S16" t="inlineStr"/>
-      <c r="T16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1640,7 +1569,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr">
         <is>
           <t>none</t>
@@ -1726,7 +1654,6 @@
           <t>unknown</t>
         </is>
       </c>
-      <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr">
         <is>
           <t>none</t>
@@ -1745,9 +1672,6 @@
           <t>GENERAL_ELEC</t>
         </is>
       </c>
-      <c r="R18" t="inlineStr"/>
-      <c r="S18" t="inlineStr"/>
-      <c r="T18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1800,7 +1724,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr">
         <is>
           <t>none</t>
@@ -1819,9 +1742,6 @@
           <t>GENERAL_ELEC</t>
         </is>
       </c>
-      <c r="R19" t="inlineStr"/>
-      <c r="S19" t="inlineStr"/>
-      <c r="T19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1850,7 +1770,6 @@
           <t>ACCO 1031; FINA 3001</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr"/>
       <c r="H20" t="b">
         <v>1</v>
       </c>
@@ -1870,7 +1789,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr">
         <is>
           <t>none</t>
@@ -1889,9 +1807,6 @@
           <t>CORE</t>
         </is>
       </c>
-      <c r="R20" t="inlineStr"/>
-      <c r="S20" t="inlineStr"/>
-      <c r="T20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1920,7 +1835,6 @@
           <t>FINA 3001</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr"/>
       <c r="H21" t="b">
         <v>1</v>
       </c>
@@ -1940,7 +1854,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr">
         <is>
           <t>none</t>
@@ -2002,7 +1915,6 @@
           <t>ACCO 1031; FINA 3001</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr"/>
       <c r="H22" t="b">
         <v>1</v>
       </c>
@@ -2022,7 +1934,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr">
         <is>
           <t>none</t>
@@ -2041,9 +1952,6 @@
           <t>CORE</t>
         </is>
       </c>
-      <c r="R22" t="inlineStr"/>
-      <c r="S22" t="inlineStr"/>
-      <c r="T22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2072,7 +1980,6 @@
           <t>FINA 3001</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr"/>
       <c r="H23" t="b">
         <v>1</v>
       </c>
@@ -2092,7 +1999,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr">
         <is>
           <t>none</t>
@@ -2154,7 +2060,6 @@
           <t>FINA 3001</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr"/>
       <c r="H24" t="b">
         <v>1</v>
       </c>
@@ -2174,7 +2079,6 @@
           <t>low</t>
         </is>
       </c>
-      <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr">
         <is>
           <t>none</t>
@@ -2236,7 +2140,6 @@
           <t>FINA 3001</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr"/>
       <c r="H25" t="b">
         <v>1</v>
       </c>
@@ -2256,7 +2159,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M25" t="inlineStr"/>
       <c r="N25" t="inlineStr">
         <is>
           <t>none</t>
@@ -2318,7 +2220,6 @@
           <t>FINA 3001</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr"/>
       <c r="H26" t="b">
         <v>1</v>
       </c>
@@ -2338,7 +2239,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M26" t="inlineStr"/>
       <c r="N26" t="inlineStr">
         <is>
           <t>none</t>
@@ -2400,7 +2300,6 @@
           <t>FINA 3001</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr"/>
       <c r="H27" t="b">
         <v>1</v>
       </c>
@@ -2420,7 +2319,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr">
         <is>
           <t>none</t>
@@ -2482,7 +2380,6 @@
           <t>FINA 3001</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr"/>
       <c r="H28" t="b">
         <v>1</v>
       </c>
@@ -2502,7 +2399,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M28" t="inlineStr"/>
       <c r="N28" t="inlineStr">
         <is>
           <t>none</t>
@@ -2564,7 +2460,6 @@
           <t>FINA 3001</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr"/>
       <c r="H29" t="b">
         <v>1</v>
       </c>
@@ -2584,7 +2479,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr">
         <is>
           <t>none</t>
@@ -2646,7 +2540,6 @@
           <t>FINA 3001; FINA 4001</t>
         </is>
       </c>
-      <c r="G30" t="inlineStr"/>
       <c r="H30" t="b">
         <v>0</v>
       </c>
@@ -2666,7 +2559,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M30" t="inlineStr"/>
       <c r="N30" t="inlineStr">
         <is>
           <t>none</t>
@@ -2728,7 +2620,6 @@
           <t>FINA 3001</t>
         </is>
       </c>
-      <c r="G31" t="inlineStr"/>
       <c r="H31" t="b">
         <v>1</v>
       </c>
@@ -2748,7 +2639,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M31" t="inlineStr"/>
       <c r="N31" t="inlineStr">
         <is>
           <t>none</t>
@@ -2810,7 +2700,6 @@
           <t>FINA 3001</t>
         </is>
       </c>
-      <c r="G32" t="inlineStr"/>
       <c r="H32" t="b">
         <v>1</v>
       </c>
@@ -2830,7 +2719,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M32" t="inlineStr"/>
       <c r="N32" t="inlineStr">
         <is>
           <t>none</t>
@@ -2916,7 +2804,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M33" t="inlineStr"/>
       <c r="N33" t="inlineStr">
         <is>
           <t>none</t>
@@ -2978,7 +2865,6 @@
           <t>FINA 3001</t>
         </is>
       </c>
-      <c r="G34" t="inlineStr"/>
       <c r="H34" t="b">
         <v>0</v>
       </c>
@@ -2998,7 +2884,6 @@
           <t>unknown</t>
         </is>
       </c>
-      <c r="M34" t="inlineStr"/>
       <c r="N34" t="inlineStr">
         <is>
           <t>none</t>
@@ -3017,9 +2902,6 @@
           <t>GENERAL_ELEC</t>
         </is>
       </c>
-      <c r="R34" t="inlineStr"/>
-      <c r="S34" t="inlineStr"/>
-      <c r="T34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3048,7 +2930,6 @@
           <t>FINA 3001</t>
         </is>
       </c>
-      <c r="G35" t="inlineStr"/>
       <c r="H35" t="b">
         <v>0</v>
       </c>
@@ -3068,7 +2949,6 @@
           <t>unknown</t>
         </is>
       </c>
-      <c r="M35" t="inlineStr"/>
       <c r="N35" t="inlineStr">
         <is>
           <t>none</t>
@@ -3087,9 +2967,6 @@
           <t>GENERAL_ELEC</t>
         </is>
       </c>
-      <c r="R35" t="inlineStr"/>
-      <c r="S35" t="inlineStr"/>
-      <c r="T35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3118,7 +2995,6 @@
           <t>FINA 4001; FINA 4011; FINA 4020; FINA 4121; FINA 4122</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr"/>
       <c r="H36" t="b">
         <v>0</v>
       </c>
@@ -3138,7 +3014,6 @@
           <t>unknown</t>
         </is>
       </c>
-      <c r="M36" t="inlineStr"/>
       <c r="N36" t="inlineStr">
         <is>
           <t>none</t>
@@ -3157,9 +3032,6 @@
           <t>GENERAL_ELEC</t>
         </is>
       </c>
-      <c r="R36" t="inlineStr"/>
-      <c r="S36" t="inlineStr"/>
-      <c r="T36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -3188,7 +3060,6 @@
           <t>FINA 3001</t>
         </is>
       </c>
-      <c r="G37" t="inlineStr"/>
       <c r="H37" t="b">
         <v>1</v>
       </c>
@@ -3208,7 +3079,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M37" t="inlineStr"/>
       <c r="N37" t="inlineStr">
         <is>
           <t>none</t>
@@ -3237,7 +3107,6 @@
           <t>BUS_ELEC_4</t>
         </is>
       </c>
-      <c r="T37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -3380,7 +3249,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M39" t="inlineStr"/>
       <c r="N39" t="inlineStr">
         <is>
           <t>none</t>
@@ -3442,7 +3310,6 @@
           <t>FINA 3002; FINA 4210</t>
         </is>
       </c>
-      <c r="G40" t="inlineStr"/>
       <c r="H40" t="b">
         <v>0</v>
       </c>
@@ -3462,7 +3329,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M40" t="inlineStr"/>
       <c r="N40" t="inlineStr">
         <is>
           <t>none</t>
@@ -3524,7 +3390,6 @@
           <t>FINA 3001</t>
         </is>
       </c>
-      <c r="G41" t="inlineStr"/>
       <c r="H41" t="b">
         <v>1</v>
       </c>
@@ -3544,7 +3409,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M41" t="inlineStr"/>
       <c r="N41" t="inlineStr">
         <is>
           <t>none</t>
@@ -3606,7 +3470,6 @@
           <t>FINA 3001</t>
         </is>
       </c>
-      <c r="G42" t="inlineStr"/>
       <c r="H42" t="b">
         <v>0</v>
       </c>
@@ -3626,7 +3489,6 @@
           <t>low</t>
         </is>
       </c>
-      <c r="M42" t="inlineStr"/>
       <c r="N42" t="inlineStr">
         <is>
           <t>none</t>
@@ -3655,7 +3517,6 @@
           <t>BUS_ELEC_4</t>
         </is>
       </c>
-      <c r="T42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -3708,7 +3569,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M43" t="inlineStr"/>
       <c r="N43" t="inlineStr">
         <is>
           <t>none</t>
@@ -3737,7 +3597,6 @@
           <t>BUS_ELEC_4</t>
         </is>
       </c>
-      <c r="T43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -3790,7 +3649,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M44" t="inlineStr"/>
       <c r="N44" t="inlineStr">
         <is>
           <t>none</t>
@@ -3819,7 +3677,6 @@
           <t>BUS_ELEC_4</t>
         </is>
       </c>
-      <c r="T44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -3872,7 +3729,6 @@
           <t>high</t>
         </is>
       </c>
-      <c r="M45" t="inlineStr"/>
       <c r="N45" t="inlineStr">
         <is>
           <t>none</t>
@@ -3891,9 +3747,6 @@
           <t>GENERAL_ELEC</t>
         </is>
       </c>
-      <c r="R45" t="inlineStr"/>
-      <c r="S45" t="inlineStr"/>
-      <c r="T45" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4367,8 +4220,6 @@
       <c r="E2" t="n">
         <v>6</v>
       </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
       <c r="H2" t="b">
         <v>1</v>
       </c>
@@ -4395,7 +4246,6 @@
       <c r="E3" t="n">
         <v>2</v>
       </c>
-      <c r="F3" t="inlineStr"/>
       <c r="G3" t="n">
         <v>3000</v>
       </c>
@@ -4425,7 +4275,6 @@
       <c r="E4" t="n">
         <v>1</v>
       </c>
-      <c r="F4" t="inlineStr"/>
       <c r="G4" t="n">
         <v>3000</v>
       </c>
@@ -4455,8 +4304,6 @@
       <c r="E5" t="n">
         <v>4</v>
       </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
       <c r="H5" t="b">
         <v>1</v>
       </c>
@@ -4480,9 +4327,6 @@
       <c r="D6" t="n">
         <v>99</v>
       </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
       <c r="H6" t="b">
         <v>0</v>
       </c>
@@ -4593,4 +4437,1672 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C97"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>track_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>course_code</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>bucket_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ACCO 1030</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ACCO 1031</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>BUAD 1001</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ECON 1103</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ECON 1104</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>BUAD 1560</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>BUAD 2001</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>FINA 3001</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>FINA 3002</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>FINA 3002</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>FINA 3002</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>FINA 3002</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>FINA 3370</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>GENERAL_ELEC</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>FINA 3986</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>GENERAL_ELEC</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>FINA 4001</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>FINA 4002</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>FINA 4002</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>FINA 4002</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>FINA 4002</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>FINA 4011</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>FINA 4020</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>FINA 4020</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>FINA 4020</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>FINA 4020</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>FINA 4023</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>FINA 4023</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>FINA 4023</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>FINA 4023</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>FINA 4040</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>FINA 4040</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>FINA 4040</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>FINA 4040</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>FINA 4050</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>FINA 4050</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>FINA 4050</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>FINA 4050</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>FINA 4060</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>FINA 4060</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>FINA 4060</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>FINA 4060</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>FINA 4065</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>FINA 4065</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>FINA 4065</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>FINA 4065</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>FINA 4075</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>FINA 4075</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>FINA 4075</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>FINA 4075</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>FINA 4081</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>FINA 4081</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>FINA 4081</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>FINA 4081</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>FINA 4082</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>FINA 4082</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>FINA 4082</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>FINA 4082</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>FINA 4084</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>FINA 4084</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>FINA 4084</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>FINA 4084</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>FINA 4085</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>FINA 4085</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>FINA 4085</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>FINA 4085</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>FINA 4121</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>GENERAL_ELEC</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>FINA 4122</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>GENERAL_ELEC</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>FINA 4123</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>GENERAL_ELEC</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>FINA 4191</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>FINA 4191</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>FINA 4191</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>FINA 4210</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>FINA 4210</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>FINA 4210</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>FINA 4210</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>FINA 4211</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>FINA 4211</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>FINA 4211</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>FINA 4211</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>FINA 4212</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>FINA 4212</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>FINA 4212</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>FINA 4212</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>FINA 4931</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>FINA 4931</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>FINA 4931</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>FINA 4931</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>FINA 4953</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>FINA 4953</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>FINA 4953</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>FINA 4986</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>FINA 4986</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>FINA 4986</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>FINA 4989</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>FINA 4989</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>FIN_CHOOSE_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>FINA 4989</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>BUS_ELEC_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>FINA 4995</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>GENERAL_ELEC</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Commit remaining Phase 3 and roadmap workspace changes
</commit_message>
<xml_diff>
--- a/marquette_courses_full.xlsx
+++ b/marquette_courses_full.xlsx
@@ -4148,7 +4148,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4197,6 +4197,11 @@
           <t>allow_double_count</t>
         </is>
       </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>role</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -4223,6 +4228,11 @@
       <c r="H2" t="b">
         <v>1</v>
       </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>core</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -4251,6 +4261,11 @@
       </c>
       <c r="H3" t="b">
         <v>1</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>elective</t>
+        </is>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Implement Phase 5 program selection flow
- Add /programs catalog + declared major/track resolution

- Merge selected programs into synthetic planning scope

- Extend frontend selectors/session/rendering for program context

- Add track publish validator + new track-aware tests

- Fix npm test entrypoint for Windows
</commit_message>
<xml_diff>
--- a/marquette_courses_full.xlsx
+++ b/marquette_courses_full.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T45"/>
+  <dimension ref="A1:T65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3745,6 +3745,1006 @@
       <c r="Q45" t="inlineStr">
         <is>
           <t>GENERAL_ELEC</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>REAL 3001</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Introduction to Commercial Real Estate</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>3</v>
+      </c>
+      <c r="D46" t="n">
+        <v>3000</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>ECON 1103; ACCO 1030</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>ECON 1103;ACCO 1030</t>
+        </is>
+      </c>
+      <c r="H46" t="b">
+        <v>1</v>
+      </c>
+      <c r="I46" t="b">
+        <v>1</v>
+      </c>
+      <c r="J46" t="b">
+        <v>1</v>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>2025 Fall; 2025 Summer; 2025 Spring; 2024 Fall</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>high</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>REAL 4061</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Real Estate Modeling</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>3</v>
+      </c>
+      <c r="D47" t="n">
+        <v>4000</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>REAL 3001 or REAL 4002 or FINA 4002</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>REAL 3001 or FINA 4002</t>
+        </is>
+      </c>
+      <c r="H47" t="b">
+        <v>0</v>
+      </c>
+      <c r="I47" t="b">
+        <v>1</v>
+      </c>
+      <c r="J47" t="b">
+        <v>0</v>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>2025 Spring; 2024 Spring; 2023 Spring; 2022 Spring</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>high</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>ACCO 4040</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>International Accounting</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>3</v>
+      </c>
+      <c r="D48" t="n">
+        <v>4000</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>ACCO 4020 (may be concurrent)</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>ACCO 4020</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>may_be_concurrent</t>
+        </is>
+      </c>
+      <c r="H48" t="b">
+        <v>1</v>
+      </c>
+      <c r="I48" t="b">
+        <v>0</v>
+      </c>
+      <c r="J48" t="b">
+        <v>0</v>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>2025 Fall; 2024 Fall; 2023 Fall; 2023 Spring</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>ECON 4040</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>International Economics</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>3</v>
+      </c>
+      <c r="D49" t="n">
+        <v>4000</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>ECON 1103; ECON 1104</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>ECON 1103;ECON 1104</t>
+        </is>
+      </c>
+      <c r="H49" t="b">
+        <v>1</v>
+      </c>
+      <c r="I49" t="b">
+        <v>1</v>
+      </c>
+      <c r="J49" t="b">
+        <v>0</v>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>2025 Fall; 2024 Spring; 2023 Spring; 2021 Fall</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>ECON 4044</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Global Integration of Financial Sectors</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>3</v>
+      </c>
+      <c r="D50" t="n">
+        <v>4000</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>ECON 1103; ECON 1104</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>ECON 1103;ECON 1104</t>
+        </is>
+      </c>
+      <c r="H50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I50" t="b">
+        <v>0</v>
+      </c>
+      <c r="J50" t="b">
+        <v>0</v>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>2018 Fall; 2018 Spring; 2017 Spring; 2016 Fall</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>Not offered since 2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>FINAI 4931</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Topics in Finance-International</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>3</v>
+      </c>
+      <c r="D51" t="n">
+        <v>4000</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>FINA 3001; OIE consent</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>FINA 3001</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>enrollment_requirement</t>
+        </is>
+      </c>
+      <c r="H51" t="b">
+        <v>0</v>
+      </c>
+      <c r="I51" t="b">
+        <v>1</v>
+      </c>
+      <c r="J51" t="b">
+        <v>0</v>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>2025 Spring; 2024 Spring</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>Requires OIE consent</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>INBUI 4931</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Topics in International Business-International</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>3</v>
+      </c>
+      <c r="D52" t="n">
+        <v>4000</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>OIE consent</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>enrollment_requirement</t>
+        </is>
+      </c>
+      <c r="H52" t="b">
+        <v>0</v>
+      </c>
+      <c r="I52" t="b">
+        <v>1</v>
+      </c>
+      <c r="J52" t="b">
+        <v>1</v>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>2025 Summer; 2025 Spring; 2024 Summer; 2024 Spring</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>high</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>Requires OIE consent</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>MARK 4040</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>International Marketing</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>3</v>
+      </c>
+      <c r="D53" t="n">
+        <v>4000</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>MARK 3001</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>MARK 3001</t>
+        </is>
+      </c>
+      <c r="H53" t="b">
+        <v>1</v>
+      </c>
+      <c r="I53" t="b">
+        <v>1</v>
+      </c>
+      <c r="J53" t="b">
+        <v>0</v>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>2025 Fall; 2025 Spring; 2024 Fall; 2024 Spring</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>high</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>ACCO 3001</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Intermediate Accounting I</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>3</v>
+      </c>
+      <c r="D54" t="n">
+        <v>3000</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>ACCO 1031</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>ACCO 1031</t>
+        </is>
+      </c>
+      <c r="H54" t="b">
+        <v>1</v>
+      </c>
+      <c r="I54" t="b">
+        <v>1</v>
+      </c>
+      <c r="J54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>2025 Fall; 2025 Spring; 2024 Fall; 2024 Spring</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>high</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>ACCO 4020</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Intermediate Accounting II</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>3</v>
+      </c>
+      <c r="D55" t="n">
+        <v>4000</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>ACCO 3001</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>ACCO 3001</t>
+        </is>
+      </c>
+      <c r="H55" t="b">
+        <v>1</v>
+      </c>
+      <c r="I55" t="b">
+        <v>1</v>
+      </c>
+      <c r="J55" t="b">
+        <v>0</v>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>2025 Fall; 2025 Spring; 2024 Fall; 2024 Spring</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>high</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>ACCO 4080</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Analysis of Financial Statements</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>3</v>
+      </c>
+      <c r="D56" t="n">
+        <v>4000</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>ACCO 3001 or AIM/CBP admission</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>ACCO 3001</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>admitted_program</t>
+        </is>
+      </c>
+      <c r="H56" t="b">
+        <v>1</v>
+      </c>
+      <c r="I56" t="b">
+        <v>1</v>
+      </c>
+      <c r="J56" t="b">
+        <v>0</v>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>2025 Fall; 2025 Spring; 2024 Fall; 2024 Spring</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>high</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>Also accepts AIM/CBP admission</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>ECON 4080</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Money, Banking and Monetary Policy</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>3</v>
+      </c>
+      <c r="D57" t="n">
+        <v>4000</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>ECON 3004</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>ECON 3004</t>
+        </is>
+      </c>
+      <c r="H57" t="b">
+        <v>1</v>
+      </c>
+      <c r="I57" t="b">
+        <v>1</v>
+      </c>
+      <c r="J57" t="b">
+        <v>1</v>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>2024 Fall; 2023 Summer; 2023 Spring; 2022 Spring</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>Irregular offering schedule</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>INSY 4051</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Business Applications Development</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>3</v>
+      </c>
+      <c r="D58" t="n">
+        <v>4000</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>INSY 3001 or ACCO 4050</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>INSY 3001 or ACCO 4050</t>
+        </is>
+      </c>
+      <c r="H58" t="b">
+        <v>1</v>
+      </c>
+      <c r="I58" t="b">
+        <v>1</v>
+      </c>
+      <c r="J58" t="b">
+        <v>0</v>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>2025 Fall; 2025 Spring; 2024 Fall; 2024 Spring</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>high</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>INSY 4053</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Project Management</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>3</v>
+      </c>
+      <c r="D59" t="n">
+        <v>4000</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>INSY 3001 or ACCO 4050 or instructor consent</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>INSY 3001 or ACCO 4050</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>instructor_consent</t>
+        </is>
+      </c>
+      <c r="H59" t="b">
+        <v>1</v>
+      </c>
+      <c r="I59" t="b">
+        <v>1</v>
+      </c>
+      <c r="J59" t="b">
+        <v>0</v>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>2025 Fall; 2025 Spring; 2024 Fall; 2024 Spring</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>high</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>MARK 4094</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Professional Selling</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>3</v>
+      </c>
+      <c r="D60" t="n">
+        <v>4000</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>MARK 3001</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>MARK 3001</t>
+        </is>
+      </c>
+      <c r="H60" t="b">
+        <v>1</v>
+      </c>
+      <c r="I60" t="b">
+        <v>1</v>
+      </c>
+      <c r="J60" t="b">
+        <v>1</v>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>2025 Fall; 2025 Summer; 2025 Spring; 2024 Fall</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>high</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>REAL 4100</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Commercial Real Estate Development</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>3</v>
+      </c>
+      <c r="D61" t="n">
+        <v>4000</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>REAL 3001 or REAL 4002 or FINA 4002</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>REAL 3001 or FINA 4002</t>
+        </is>
+      </c>
+      <c r="H61" t="b">
+        <v>0</v>
+      </c>
+      <c r="I61" t="b">
+        <v>1</v>
+      </c>
+      <c r="J61" t="b">
+        <v>0</v>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>2025 Spring; 2024 Spring; 2023 Spring; 2022 Spring</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>high</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>MARK 3001</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Introduction to Marketing</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>3</v>
+      </c>
+      <c r="D62" t="n">
+        <v>3000</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Soph. stndg.; ECON 1001 or ECON 1103</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>ECON 1103</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>standing_requirement</t>
+        </is>
+      </c>
+      <c r="H62" t="b">
+        <v>1</v>
+      </c>
+      <c r="I62" t="b">
+        <v>1</v>
+      </c>
+      <c r="J62" t="b">
+        <v>1</v>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>2025 Fall; 2025 Summer; 2025 Spring; 2024 Fall</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>high</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>ECON 3004</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Intermediate Macroeconomic Analysis</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>3</v>
+      </c>
+      <c r="D63" t="n">
+        <v>3000</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>ECON 1103; ECON 1104; MATH 1400 or equiv.</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>ECON 1103;ECON 1104;MATH 1400</t>
+        </is>
+      </c>
+      <c r="H63" t="b">
+        <v>1</v>
+      </c>
+      <c r="I63" t="b">
+        <v>1</v>
+      </c>
+      <c r="J63" t="b">
+        <v>0</v>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>2025 Fall; 2025 Spring; 2024 Fall; 2024 Spring</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>high</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>INSY 3001</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Introduction to Information Systems</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>3</v>
+      </c>
+      <c r="D64" t="n">
+        <v>3000</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Soph. stndg.</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>standing_requirement</t>
+        </is>
+      </c>
+      <c r="H64" t="b">
+        <v>1</v>
+      </c>
+      <c r="I64" t="b">
+        <v>1</v>
+      </c>
+      <c r="J64" t="b">
+        <v>1</v>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>2025 Fall; 2025 Summer; 2025 Spring; 2024 Fall</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>high</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>ACCO 4050</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Accounting Information Systems</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>3</v>
+      </c>
+      <c r="D65" t="n">
+        <v>4000</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>ACCO 1031</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>ACCO 1031</t>
+        </is>
+      </c>
+      <c r="H65" t="b">
+        <v>1</v>
+      </c>
+      <c r="I65" t="b">
+        <v>1</v>
+      </c>
+      <c r="J65" t="b">
+        <v>0</v>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>2025 Fall; 2025 Summer; 2024 Fall; 2024 Summer</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>high</t>
         </is>
       </c>
     </row>
@@ -4067,7 +5067,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4091,6 +5091,16 @@
           <t>active</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>kind</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>parent_major_id</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -4106,6 +5116,12 @@
       <c r="C2" t="b">
         <v>1</v>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>major</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -4121,6 +5137,16 @@
       <c r="C3" t="b">
         <v>0</v>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>track</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -4135,6 +5161,16 @@
       </c>
       <c r="C4" t="b">
         <v>0</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>track</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>FIN_MAJOR</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -4148,7 +5184,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4344,6 +5380,125 @@
       </c>
       <c r="H6" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>FP_CONC</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>FP_CORE</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Financial Planning Required</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>7</v>
+      </c>
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>core</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>CB_CORE</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Commercial Banking Required</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>9</v>
+      </c>
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>core</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>CB_INTL</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>International Requirement</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>CB_ELEC</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Commercial Banking Elective</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2</v>
+      </c>
+      <c r="H10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>elective</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -4460,7 +5615,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C97"/>
+  <dimension ref="A1:C136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6117,6 +7272,669 @@
         </is>
       </c>
     </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>FP_CONC</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>FINA 3001</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>FP_CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>FP_CONC</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>FINA 4001</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>FP_CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>FP_CONC</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>FINA 4011</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>FP_CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>FP_CONC</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>FINA 4020</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>FP_CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>FP_CONC</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>FINA 4121</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>FP_CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>FP_CONC</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>FINA 4122</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>FP_CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>FP_CONC</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>FINA 4123</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>FP_CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>FINA 3001</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>CB_CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>FINA 3002</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>CB_CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>FINA 4001</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>CB_CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>FINA 4011</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>CB_CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>FINA 4050</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>CB_CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>REAL 4061</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>CB_CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>FINA 4210</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>CB_CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>FINA 4211</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>CB_CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>FINA 4212</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>CB_CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>REAL 3001</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>CB_CORE</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>ACCO 4040</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>CB_INTL</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>ECON 4040</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>CB_INTL</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>ECON 4044</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>CB_INTL</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>FINA 4040</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>CB_INTL</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>FINAI 4931</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>CB_INTL</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>INBUI 4931</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>CB_INTL</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>MARK 4040</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>CB_INTL</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>ACCO 3001</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>CB_ELEC</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>ACCO 4020</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>CB_ELEC</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>ACCO 4080</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>CB_ELEC</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>FINA 4002</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>CB_ELEC</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>FINA 4065</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>CB_ELEC</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>FINA 4075</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>CB_ELEC</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>FINA 4081</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>CB_ELEC</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>FINA 4082</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>CB_ELEC</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>FINA 4084</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>CB_ELEC</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>ECON 4080</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>CB_ELEC</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>INSY 4051</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>CB_ELEC</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>INSY 4053</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>CB_ELEC</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>MARK 4094</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>CB_ELEC</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>REAL 4100</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>CB_ELEC</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>CB_CONC</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>REAL 4061</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>CB_ELEC</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Stabilize course search and reorganize test suites
</commit_message>
<xml_diff>
--- a/marquette_courses_full.xlsx
+++ b/marquette_courses_full.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T65"/>
+  <dimension ref="A1:S65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,25 +504,20 @@
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>prereq_tier</t>
+          <t>bucket1</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>bucket1</t>
+          <t>bucket2</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>bucket2</t>
+          <t>bucket3</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
-        <is>
-          <t>bucket3</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
         <is>
           <t>bucket4</t>
         </is>
@@ -584,11 +579,6 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>level_0</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
           <t>BUS_ELEC_4</t>
         </is>
       </c>
@@ -649,11 +639,6 @@
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>level_1</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
           <t>BUS_ELEC_4</t>
         </is>
       </c>
@@ -719,11 +704,6 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>level_0</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
           <t>BUS_ELEC_4</t>
         </is>
       </c>
@@ -782,11 +762,6 @@
       <c r="O5" t="n">
         <v>0</v>
       </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>level_0</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -844,11 +819,6 @@
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>level_0</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
           <t>BUS_ELEC_4</t>
         </is>
       </c>
@@ -909,11 +879,6 @@
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>level_1</t>
-        </is>
-      </c>
-      <c r="Q7" t="inlineStr">
-        <is>
           <t>BUS_ELEC_4</t>
         </is>
       </c>
@@ -977,11 +942,6 @@
       <c r="O8" t="n">
         <v>0</v>
       </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>level_0</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1042,11 +1002,6 @@
       <c r="O9" t="n">
         <v>0</v>
       </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>level_0</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1107,11 +1062,6 @@
       <c r="O10" t="n">
         <v>1</v>
       </c>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>level_1</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1172,11 +1122,6 @@
       <c r="O11" t="n">
         <v>1</v>
       </c>
-      <c r="P11" t="inlineStr">
-        <is>
-          <t>level_1</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1234,11 +1179,6 @@
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>level_2</t>
-        </is>
-      </c>
-      <c r="Q12" t="inlineStr">
-        <is>
           <t>BUS_ELEC_4</t>
         </is>
       </c>
@@ -1304,11 +1244,6 @@
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>level_1</t>
-        </is>
-      </c>
-      <c r="Q13" t="inlineStr">
-        <is>
           <t>BUS_ELEC_4</t>
         </is>
       </c>
@@ -1372,11 +1307,6 @@
       <c r="O14" t="n">
         <v>0</v>
       </c>
-      <c r="P14" t="inlineStr">
-        <is>
-          <t>level_0</t>
-        </is>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1437,11 +1367,6 @@
       <c r="O15" t="n">
         <v>1</v>
       </c>
-      <c r="P15" t="inlineStr">
-        <is>
-          <t>level_1</t>
-        </is>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1509,11 +1434,6 @@
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>level_2</t>
-        </is>
-      </c>
-      <c r="Q16" t="inlineStr">
-        <is>
           <t>CORE</t>
         </is>
       </c>
@@ -1579,25 +1499,20 @@
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>level_3</t>
+          <t>CORE</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>CORE</t>
+          <t>FIN_CHOOSE_2</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>FIN_CHOOSE_2</t>
+          <t>FIN_CHOOSE_1</t>
         </is>
       </c>
       <c r="S17" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="T17" t="inlineStr">
         <is>
           <t>BUS_ELEC_4</t>
         </is>
@@ -1664,11 +1579,6 @@
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>level_0</t>
-        </is>
-      </c>
-      <c r="Q18" t="inlineStr">
-        <is>
           <t>GENERAL_ELEC</t>
         </is>
       </c>
@@ -1734,11 +1644,6 @@
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>level_3</t>
-        </is>
-      </c>
-      <c r="Q19" t="inlineStr">
-        <is>
           <t>GENERAL_ELEC</t>
         </is>
       </c>
@@ -1799,11 +1704,6 @@
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>level_3</t>
-        </is>
-      </c>
-      <c r="Q20" t="inlineStr">
-        <is>
           <t>CORE</t>
         </is>
       </c>
@@ -1864,25 +1764,20 @@
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>level_3</t>
+          <t>CORE</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>CORE</t>
+          <t>FIN_CHOOSE_2</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
         <is>
-          <t>FIN_CHOOSE_2</t>
+          <t>FIN_CHOOSE_1</t>
         </is>
       </c>
       <c r="S21" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="T21" t="inlineStr">
         <is>
           <t>BUS_ELEC_4</t>
         </is>
@@ -1944,11 +1839,6 @@
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>level_3</t>
-        </is>
-      </c>
-      <c r="Q22" t="inlineStr">
-        <is>
           <t>CORE</t>
         </is>
       </c>
@@ -2009,25 +1899,20 @@
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>level_3</t>
+          <t>CORE</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>CORE</t>
+          <t>FIN_CHOOSE_2</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
         <is>
-          <t>FIN_CHOOSE_2</t>
+          <t>FIN_CHOOSE_1</t>
         </is>
       </c>
       <c r="S23" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="T23" t="inlineStr">
         <is>
           <t>BUS_ELEC_4</t>
         </is>
@@ -2089,25 +1974,20 @@
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>level_3</t>
+          <t>CORE</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>CORE</t>
+          <t>FIN_CHOOSE_2</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
         <is>
-          <t>FIN_CHOOSE_2</t>
+          <t>FIN_CHOOSE_1</t>
         </is>
       </c>
       <c r="S24" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="T24" t="inlineStr">
         <is>
           <t>BUS_ELEC_4</t>
         </is>
@@ -2169,25 +2049,20 @@
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>level_3</t>
+          <t>CORE</t>
         </is>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>CORE</t>
+          <t>FIN_CHOOSE_2</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
         <is>
-          <t>FIN_CHOOSE_2</t>
+          <t>FIN_CHOOSE_1</t>
         </is>
       </c>
       <c r="S25" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="T25" t="inlineStr">
         <is>
           <t>BUS_ELEC_4</t>
         </is>
@@ -2249,25 +2124,20 @@
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>level_3</t>
+          <t>CORE</t>
         </is>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>CORE</t>
+          <t>FIN_CHOOSE_2</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
         <is>
-          <t>FIN_CHOOSE_2</t>
+          <t>FIN_CHOOSE_1</t>
         </is>
       </c>
       <c r="S26" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="T26" t="inlineStr">
         <is>
           <t>BUS_ELEC_4</t>
         </is>
@@ -2329,25 +2199,20 @@
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>level_3</t>
+          <t>CORE</t>
         </is>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>CORE</t>
+          <t>FIN_CHOOSE_2</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
         <is>
-          <t>FIN_CHOOSE_2</t>
+          <t>FIN_CHOOSE_1</t>
         </is>
       </c>
       <c r="S27" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="T27" t="inlineStr">
         <is>
           <t>BUS_ELEC_4</t>
         </is>
@@ -2409,25 +2274,20 @@
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>level_3</t>
+          <t>CORE</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>CORE</t>
+          <t>FIN_CHOOSE_2</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
         <is>
-          <t>FIN_CHOOSE_2</t>
+          <t>FIN_CHOOSE_1</t>
         </is>
       </c>
       <c r="S28" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="T28" t="inlineStr">
         <is>
           <t>BUS_ELEC_4</t>
         </is>
@@ -2489,25 +2349,20 @@
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>level_3</t>
+          <t>CORE</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>CORE</t>
+          <t>FIN_CHOOSE_2</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
         <is>
-          <t>FIN_CHOOSE_2</t>
+          <t>FIN_CHOOSE_1</t>
         </is>
       </c>
       <c r="S29" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="T29" t="inlineStr">
         <is>
           <t>BUS_ELEC_4</t>
         </is>
@@ -2569,25 +2424,20 @@
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>level_4</t>
+          <t>CORE</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>CORE</t>
+          <t>FIN_CHOOSE_2</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
         <is>
-          <t>FIN_CHOOSE_2</t>
+          <t>FIN_CHOOSE_1</t>
         </is>
       </c>
       <c r="S30" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="T30" t="inlineStr">
         <is>
           <t>BUS_ELEC_4</t>
         </is>
@@ -2649,25 +2499,20 @@
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>level_3</t>
+          <t>CORE</t>
         </is>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>CORE</t>
+          <t>FIN_CHOOSE_2</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
         <is>
-          <t>FIN_CHOOSE_2</t>
+          <t>FIN_CHOOSE_1</t>
         </is>
       </c>
       <c r="S31" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="T31" t="inlineStr">
         <is>
           <t>BUS_ELEC_4</t>
         </is>
@@ -2729,25 +2574,20 @@
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>level_3</t>
+          <t>CORE</t>
         </is>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>CORE</t>
+          <t>FIN_CHOOSE_2</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
         <is>
-          <t>FIN_CHOOSE_2</t>
+          <t>FIN_CHOOSE_1</t>
         </is>
       </c>
       <c r="S32" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="T32" t="inlineStr">
         <is>
           <t>BUS_ELEC_4</t>
         </is>
@@ -2814,25 +2654,20 @@
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>level_4</t>
+          <t>CORE</t>
         </is>
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>CORE</t>
+          <t>FIN_CHOOSE_2</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
         <is>
-          <t>FIN_CHOOSE_2</t>
+          <t>FIN_CHOOSE_1</t>
         </is>
       </c>
       <c r="S33" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="T33" t="inlineStr">
         <is>
           <t>BUS_ELEC_4</t>
         </is>
@@ -2894,11 +2729,6 @@
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>level_3</t>
-        </is>
-      </c>
-      <c r="Q34" t="inlineStr">
-        <is>
           <t>GENERAL_ELEC</t>
         </is>
       </c>
@@ -2959,11 +2789,6 @@
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>level_3</t>
-        </is>
-      </c>
-      <c r="Q35" t="inlineStr">
-        <is>
           <t>GENERAL_ELEC</t>
         </is>
       </c>
@@ -3024,11 +2849,6 @@
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>level_4</t>
-        </is>
-      </c>
-      <c r="Q36" t="inlineStr">
-        <is>
           <t>GENERAL_ELEC</t>
         </is>
       </c>
@@ -3089,20 +2909,15 @@
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>level_3</t>
+          <t>CORE</t>
         </is>
       </c>
       <c r="Q37" t="inlineStr">
         <is>
-          <t>CORE</t>
+          <t>FIN_CHOOSE_2</t>
         </is>
       </c>
       <c r="R37" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_2</t>
-        </is>
-      </c>
-      <c r="S37" t="inlineStr">
         <is>
           <t>BUS_ELEC_4</t>
         </is>
@@ -3174,25 +2989,20 @@
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>level_3</t>
+          <t>CORE</t>
         </is>
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>CORE</t>
+          <t>FIN_CHOOSE_2</t>
         </is>
       </c>
       <c r="R38" t="inlineStr">
         <is>
-          <t>FIN_CHOOSE_2</t>
+          <t>FIN_CHOOSE_1</t>
         </is>
       </c>
       <c r="S38" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="T38" t="inlineStr">
         <is>
           <t>BUS_ELEC_4</t>
         </is>
@@ -3259,25 +3069,20 @@
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>level_4</t>
+          <t>CORE</t>
         </is>
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>CORE</t>
+          <t>FIN_CHOOSE_2</t>
         </is>
       </c>
       <c r="R39" t="inlineStr">
         <is>
-          <t>FIN_CHOOSE_2</t>
+          <t>FIN_CHOOSE_1</t>
         </is>
       </c>
       <c r="S39" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="T39" t="inlineStr">
         <is>
           <t>BUS_ELEC_4</t>
         </is>
@@ -3339,25 +3144,20 @@
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>level_4</t>
+          <t>CORE</t>
         </is>
       </c>
       <c r="Q40" t="inlineStr">
         <is>
-          <t>CORE</t>
+          <t>FIN_CHOOSE_2</t>
         </is>
       </c>
       <c r="R40" t="inlineStr">
         <is>
-          <t>FIN_CHOOSE_2</t>
+          <t>FIN_CHOOSE_1</t>
         </is>
       </c>
       <c r="S40" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="T40" t="inlineStr">
         <is>
           <t>BUS_ELEC_4</t>
         </is>
@@ -3419,25 +3219,20 @@
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>level_3</t>
+          <t>CORE</t>
         </is>
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>CORE</t>
+          <t>FIN_CHOOSE_2</t>
         </is>
       </c>
       <c r="R41" t="inlineStr">
         <is>
-          <t>FIN_CHOOSE_2</t>
+          <t>FIN_CHOOSE_1</t>
         </is>
       </c>
       <c r="S41" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_1</t>
-        </is>
-      </c>
-      <c r="T41" t="inlineStr">
         <is>
           <t>BUS_ELEC_4</t>
         </is>
@@ -3499,20 +3294,15 @@
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>level_3</t>
+          <t>CORE</t>
         </is>
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>CORE</t>
+          <t>FIN_CHOOSE_2</t>
         </is>
       </c>
       <c r="R42" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_2</t>
-        </is>
-      </c>
-      <c r="S42" t="inlineStr">
         <is>
           <t>BUS_ELEC_4</t>
         </is>
@@ -3579,20 +3369,15 @@
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>level_4</t>
+          <t>CORE</t>
         </is>
       </c>
       <c r="Q43" t="inlineStr">
         <is>
-          <t>CORE</t>
+          <t>FIN_CHOOSE_2</t>
         </is>
       </c>
       <c r="R43" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_2</t>
-        </is>
-      </c>
-      <c r="S43" t="inlineStr">
         <is>
           <t>BUS_ELEC_4</t>
         </is>
@@ -3659,20 +3444,15 @@
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>level_3</t>
+          <t>CORE</t>
         </is>
       </c>
       <c r="Q44" t="inlineStr">
         <is>
-          <t>CORE</t>
+          <t>FIN_CHOOSE_2</t>
         </is>
       </c>
       <c r="R44" t="inlineStr">
-        <is>
-          <t>FIN_CHOOSE_2</t>
-        </is>
-      </c>
-      <c r="S44" t="inlineStr">
         <is>
           <t>BUS_ELEC_4</t>
         </is>
@@ -3739,11 +3519,6 @@
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>level_0</t>
-        </is>
-      </c>
-      <c r="Q45" t="inlineStr">
-        <is>
           <t>GENERAL_ELEC</t>
         </is>
       </c>
@@ -3794,6 +3569,9 @@
           <t>high</t>
         </is>
       </c>
+      <c r="O46" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -3841,6 +3619,9 @@
           <t>high</t>
         </is>
       </c>
+      <c r="O47" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -3893,6 +3674,9 @@
           <t>medium</t>
         </is>
       </c>
+      <c r="O48" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -3940,6 +3724,9 @@
           <t>medium</t>
         </is>
       </c>
+      <c r="O49" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -3992,6 +3779,9 @@
           <t>Not offered since 2018</t>
         </is>
       </c>
+      <c r="O50" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -4049,6 +3839,9 @@
           <t>Requires OIE consent</t>
         </is>
       </c>
+      <c r="O51" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -4106,6 +3899,9 @@
           <t>Requires OIE consent</t>
         </is>
       </c>
+      <c r="O52" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -4153,6 +3949,9 @@
           <t>high</t>
         </is>
       </c>
+      <c r="O53" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -4200,6 +3999,9 @@
           <t>high</t>
         </is>
       </c>
+      <c r="O54" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -4247,6 +4049,9 @@
           <t>high</t>
         </is>
       </c>
+      <c r="O55" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -4304,6 +4109,9 @@
           <t>Also accepts AIM/CBP admission</t>
         </is>
       </c>
+      <c r="O56" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -4356,6 +4164,9 @@
           <t>Irregular offering schedule</t>
         </is>
       </c>
+      <c r="O57" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -4403,6 +4214,9 @@
           <t>high</t>
         </is>
       </c>
+      <c r="O58" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -4455,6 +4269,9 @@
           <t>high</t>
         </is>
       </c>
+      <c r="O59" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -4502,6 +4319,9 @@
           <t>high</t>
         </is>
       </c>
+      <c r="O60" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -4549,6 +4369,9 @@
           <t>high</t>
         </is>
       </c>
+      <c r="O61" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -4601,6 +4424,9 @@
           <t>high</t>
         </is>
       </c>
+      <c r="O62" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -4648,6 +4474,9 @@
           <t>high</t>
         </is>
       </c>
+      <c r="O63" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -4700,6 +4529,9 @@
           <t>high</t>
         </is>
       </c>
+      <c r="O64" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -4746,6 +4578,9 @@
         <is>
           <t>high</t>
         </is>
+      </c>
+      <c r="O65" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -5121,7 +4956,6 @@
           <t>major</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">

</xml_diff>

<commit_message>
Improve prerequisite assumptions and fix source prereq data
</commit_message>
<xml_diff>
--- a/marquette_courses_full.xlsx
+++ b/marquette_courses_full.xlsx
@@ -1087,7 +1087,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>MATH 1200</t>
+          <t>MATH 1400</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1392,7 +1392,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>ACCO 1031</t>
+          <t>ACCO 1031;ECON 1103</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">

</xml_diff>